<commit_message>
pavani new change 1
pavani new change 1
</commit_message>
<xml_diff>
--- a/trigger info.xlsx
+++ b/trigger info.xlsx
@@ -363,10 +363,10 @@
     <t>request_values_table</t>
   </si>
   <si>
-    <t>changed new</t>
-  </si>
-  <si>
-    <t>pavani new</t>
+    <t>changed new 1</t>
+  </si>
+  <si>
+    <t>pavani new 1</t>
   </si>
 </sst>
 </file>

</xml_diff>